<commit_message>
Rewrite humanized manuscript to reduce AI detection score
Deep rewrite of all prose-heavy sections (Abstract, Introduction, Related Work,
Discussion, Conclusion, Results narration) focusing on perplexity and burstiness
rather than surface pattern removal. Updated experiment results, figures, and
model training summaries across both datasets.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/scene_classification/results/tables/performance/cross_dataset_comparison.xlsx
+++ b/scene_classification/results/tables/performance/cross_dataset_comparison.xlsx
@@ -491,16 +491,16 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>0.9881481481481481</v>
+        <v>0.987037037037037</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.9878372361608717</v>
+        <v>0.9865022853476677</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.9928571428571429</v>
+        <v>0.9952380952380953</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.9929079824550209</v>
+        <v>0.9952351171863368</v>
       </c>
     </row>
     <row r="3">
@@ -510,16 +510,16 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>0.9812962962962963</v>
+        <v>0.9890740740740741</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.9805931789193008</v>
+        <v>0.9887031337958833</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.9880952380952381</v>
+        <v>0.9928571428571429</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.9881998953427524</v>
+        <v>0.9928526757795052</v>
       </c>
     </row>
     <row r="4">
@@ -529,16 +529,16 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.9846296296296296</v>
+        <v>0.9896296296296296</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.9840817349260412</v>
+        <v>0.9893331952174449</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.9928571428571429</v>
+        <v>0.9904761904761905</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.992852675779505</v>
+        <v>0.9904612778260312</v>
       </c>
     </row>
     <row r="5">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.9853703703703703</v>
+        <v>0.9875925925925926</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>0.9852531981524704</v>
+        <v>0.9870486448163949</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0.9952380952380953</v>
@@ -570,13 +570,13 @@
         <v>0.9898148148148148</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>0.9893665329922848</v>
+        <v>0.9895197400624811</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.9976190476190476</v>
+        <v>0.9952380952380953</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.9976175585931684</v>
+        <v>0.9952351171863366</v>
       </c>
     </row>
     <row r="7">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.9890740740740741</v>
+        <v>0.9872222222222222</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.9889196143013048</v>
+        <v>0.9869984774436796</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.9952380952380953</v>
+        <v>0.9809523809523809</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.9952351171863368</v>
+        <v>0.9809002756089702</v>
       </c>
     </row>
     <row r="8">
@@ -605,16 +605,16 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0.99</v>
+        <v>0.9901851851851852</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0.9896106784688776</v>
+        <v>0.9898819612599488</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.9976190476190476</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.9904627668519106</v>
+        <v>0.9976175585931684</v>
       </c>
     </row>
     <row r="9">
@@ -624,16 +624,16 @@
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>0.9905555555555555</v>
+        <v>0.9911111111111112</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>0.9902213658271904</v>
+        <v>0.9908032995990874</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>0.9952380952380953</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.9952904238618524</v>
+        <v>0.9952351171863368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>